<commit_message>
build: change name to sheets
</commit_message>
<xml_diff>
--- a/src/files/records-example.xlsx
+++ b/src/files/records-example.xlsx
@@ -5,21 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bowie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bowie\Desktop\mgmt-records\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2460"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="general" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">General!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">general!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:H16"/>
     </sheetView>
   </sheetViews>
@@ -846,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>